<commit_message>
Changed 1% modifier on units vs units to 5%
</commit_message>
<xml_diff>
--- a/assets/UnitMod.xlsx
+++ b/assets/UnitMod.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\gameassets\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\tribalhero\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -891,7 +891,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
       <pane ySplit="7200"/>
-      <selection activeCell="D15" sqref="D15:V30"/>
+      <selection activeCell="R29" sqref="R29"/>
       <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
@@ -1491,10 +1491,10 @@
         <v>0.01</v>
       </c>
       <c r="R21" s="3">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="S21" s="3">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="T21" s="3">
         <v>0.01</v>
@@ -1556,10 +1556,10 @@
         <v>0.01</v>
       </c>
       <c r="R22" s="3">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="S22" s="3">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="T22" s="3">
         <v>0.01</v>
@@ -1816,10 +1816,10 @@
         <v>0.01</v>
       </c>
       <c r="R26" s="3">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="S26" s="3">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="T26" s="3">
         <v>0.01</v>
@@ -2011,10 +2011,10 @@
         <v>0.01</v>
       </c>
       <c r="R29" s="3">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="S29" s="3">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="T29" s="3">
         <v>0.01</v>
@@ -2560,11 +2560,11 @@
       </c>
       <c r="R43" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>-1.24</v>
+        <v>-1.2</v>
       </c>
       <c r="S43" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>-0.24</v>
+        <v>-0.2</v>
       </c>
       <c r="T43" s="3">
         <f t="shared" ca="1" si="5"/>
@@ -2627,11 +2627,11 @@
       </c>
       <c r="R44" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>-1.24</v>
+        <v>-1.2</v>
       </c>
       <c r="S44" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>-0.24</v>
+        <v>-0.2</v>
       </c>
       <c r="T44" s="3">
         <f t="shared" ca="1" si="6"/>
@@ -2871,11 +2871,11 @@
       </c>
       <c r="M48" s="3">
         <f t="shared" ca="1" si="10"/>
-        <v>1.24</v>
+        <v>1.2</v>
       </c>
       <c r="N48" s="3">
         <f t="shared" ca="1" si="10"/>
-        <v>1.24</v>
+        <v>1.2</v>
       </c>
       <c r="O48" s="3">
         <f t="shared" ca="1" si="10"/>
@@ -2895,7 +2895,7 @@
       </c>
       <c r="S48" s="3">
         <f t="shared" ca="1" si="10"/>
-        <v>-0.99</v>
+        <v>-0.95</v>
       </c>
       <c r="T48" s="3">
         <f t="shared" ca="1" si="10"/>
@@ -3529,11 +3529,11 @@
       </c>
       <c r="R62" s="3">
         <f t="shared" si="18"/>
-        <v>0.21</v>
+        <v>1.05</v>
       </c>
       <c r="S62" s="3">
         <f t="shared" si="18"/>
-        <v>0.21</v>
+        <v>1.05</v>
       </c>
       <c r="T62" s="3">
         <f t="shared" si="18"/>
@@ -3595,11 +3595,11 @@
       </c>
       <c r="R63" s="3">
         <f t="shared" si="19"/>
-        <v>0.21</v>
+        <v>1.05</v>
       </c>
       <c r="S63" s="3">
         <f t="shared" si="19"/>
-        <v>0.21</v>
+        <v>1.05</v>
       </c>
       <c r="T63" s="3">
         <f t="shared" si="19"/>
@@ -3855,11 +3855,11 @@
       </c>
       <c r="R67" s="3">
         <f t="shared" si="23"/>
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="S67" s="3">
         <f t="shared" si="23"/>
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="T67" s="3">
         <f t="shared" si="23"/>
@@ -4493,11 +4493,11 @@
       </c>
       <c r="R80" s="9">
         <f t="shared" ca="1" si="32"/>
-        <v>333.33333333333337</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="S80" s="9">
         <f t="shared" ca="1" si="32"/>
-        <v>952.38095238095241</v>
+        <v>190.47619047619048</v>
       </c>
       <c r="T80" s="9">
         <f t="shared" ca="1" si="32"/>
@@ -4505,7 +4505,7 @@
       </c>
       <c r="U80" s="9">
         <f t="shared" ca="1" si="27"/>
-        <v>1566.747252747253</v>
+        <v>1487.6263736263738</v>
       </c>
     </row>
     <row r="81" spans="4:22" x14ac:dyDescent="0.25">
@@ -4563,11 +4563,11 @@
       </c>
       <c r="R81" s="9">
         <f t="shared" ca="1" si="33"/>
-        <v>333.33333333333337</v>
+        <v>66.666666666666657</v>
       </c>
       <c r="S81" s="9">
         <f t="shared" ca="1" si="33"/>
-        <v>952.38095238095241</v>
+        <v>190.47619047619048</v>
       </c>
       <c r="T81" s="9">
         <f t="shared" ca="1" si="33"/>
@@ -4575,7 +4575,7 @@
       </c>
       <c r="U81" s="9">
         <f t="shared" ca="1" si="27"/>
-        <v>1566.832722832723</v>
+        <v>1487.711843711844</v>
       </c>
     </row>
     <row r="82" spans="4:22" x14ac:dyDescent="0.25">
@@ -4839,11 +4839,11 @@
       </c>
       <c r="R85" s="9">
         <f t="shared" ca="1" si="37"/>
-        <v>700</v>
+        <v>140</v>
       </c>
       <c r="S85" s="9">
         <f t="shared" ca="1" si="37"/>
-        <v>2000</v>
+        <v>400</v>
       </c>
       <c r="T85" s="9">
         <f t="shared" ca="1" si="37"/>
@@ -4851,7 +4851,7 @@
       </c>
       <c r="U85" s="9">
         <f t="shared" ca="1" si="27"/>
-        <v>3290.2461538461534</v>
+        <v>3124.0923076923073</v>
       </c>
     </row>
     <row r="86" spans="4:22" x14ac:dyDescent="0.25">
@@ -5038,11 +5038,11 @@
       </c>
       <c r="R88" s="16">
         <f t="shared" ca="1" si="40"/>
-        <v>222.7820512820513</v>
+        <v>138.67948717948718</v>
       </c>
       <c r="S88" s="16">
         <f t="shared" ca="1" si="40"/>
-        <v>637.44322344322347</v>
+        <v>397.15018315018312</v>
       </c>
       <c r="T88" s="16">
         <f t="shared" ca="1" si="40"/>
@@ -5050,7 +5050,7 @@
       </c>
       <c r="U88" s="9">
         <f t="shared" ca="1" si="27"/>
-        <v>1975.7821874706492</v>
+        <v>1950.8286794402179</v>
       </c>
     </row>
     <row r="91" spans="4:22" x14ac:dyDescent="0.25">
@@ -5545,11 +5545,11 @@
       </c>
       <c r="R99" s="9">
         <f t="shared" ca="1" si="46"/>
-        <v>-327.73333333333335</v>
+        <v>-61.066666666666656</v>
       </c>
       <c r="S99" s="9">
         <f t="shared" ca="1" si="46"/>
-        <v>-924.38095238095241</v>
+        <v>-162.47619047619048</v>
       </c>
       <c r="T99" s="9">
         <f t="shared" ca="1" si="46"/>
@@ -5614,11 +5614,11 @@
       </c>
       <c r="R100" s="9">
         <f t="shared" ca="1" si="47"/>
-        <v>-326.93333333333339</v>
+        <v>-60.266666666666659</v>
       </c>
       <c r="S100" s="9">
         <f t="shared" ca="1" si="47"/>
-        <v>-920.38095238095241</v>
+        <v>-158.47619047619048</v>
       </c>
       <c r="T100" s="9">
         <f t="shared" ca="1" si="47"/>
@@ -5866,11 +5866,11 @@
       </c>
       <c r="M104" s="9">
         <f t="shared" ca="1" si="51"/>
-        <v>327.73333333333335</v>
+        <v>61.066666666666656</v>
       </c>
       <c r="N104" s="9">
         <f t="shared" ca="1" si="51"/>
-        <v>326.93333333333339</v>
+        <v>60.266666666666659</v>
       </c>
       <c r="O104" s="9">
         <f t="shared" ca="1" si="51"/>
@@ -5890,7 +5890,7 @@
       </c>
       <c r="S104" s="9">
         <f t="shared" ca="1" si="51"/>
-        <v>-1993</v>
+        <v>-393</v>
       </c>
       <c r="T104" s="9">
         <f t="shared" ca="1" si="51"/>
@@ -5935,11 +5935,11 @@
       </c>
       <c r="M105" s="9">
         <f t="shared" ca="1" si="52"/>
-        <v>924.38095238095241</v>
+        <v>162.47619047619048</v>
       </c>
       <c r="N105" s="9">
         <f t="shared" ca="1" si="52"/>
-        <v>920.38095238095241</v>
+        <v>158.47619047619048</v>
       </c>
       <c r="O105" s="9">
         <f t="shared" ca="1" si="52"/>
@@ -5955,7 +5955,7 @@
       </c>
       <c r="R105" s="9">
         <f t="shared" ca="1" si="52"/>
-        <v>1993</v>
+        <v>393</v>
       </c>
       <c r="S105" s="9">
         <f t="shared" ca="1" si="52"/>
@@ -6346,11 +6346,11 @@
       </c>
       <c r="P116" s="6">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="Q116" s="6">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="R116" s="6">
         <f t="shared" si="57"/>
@@ -6563,11 +6563,11 @@
       </c>
       <c r="P121" s="6">
         <f t="shared" si="59"/>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="Q121" s="6">
         <f t="shared" si="59"/>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="R121" s="6">
         <f t="shared" si="59"/>
@@ -7041,11 +7041,11 @@
       </c>
       <c r="P133" s="1">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="Q133" s="1">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="R133" s="1">
         <f t="shared" si="63"/>
@@ -7257,11 +7257,11 @@
       </c>
       <c r="P137" s="1">
         <f t="shared" si="66"/>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="Q137" s="1">
         <f t="shared" si="66"/>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="R137" s="1">
         <f t="shared" si="66"/>
@@ -7419,11 +7419,11 @@
       </c>
       <c r="P140" s="1">
         <f t="shared" si="66"/>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="Q140" s="1">
         <f t="shared" si="66"/>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="R140" s="1">
         <f t="shared" si="66"/>

</xml_diff>